<commit_message>
add duckdb, split app into ui and server
</commit_message>
<xml_diff>
--- a/shiny/shinydata/file_info.xlsx
+++ b/shiny/shinydata/file_info.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Documents/WORKSPACE/osa-mbon/shiny/shinydata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DBF6C0-539D-DC4A-AFCB-B5D1A63BCD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE09C62-4A36-3444-85A0-2E2F6EFB8B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="780" windowWidth="23820" windowHeight="16940" activeTab="1" xr2:uid="{4F810807-4535-204B-9DA7-8B6B8FE1873E}"/>
+    <workbookView xWindow="920" yWindow="780" windowWidth="23820" windowHeight="16940" xr2:uid="{4F810807-4535-204B-9DA7-8B6B8FE1873E}"/>
   </bookViews>
   <sheets>
     <sheet name="acoustic_indices" sheetId="1" r:id="rId1"/>
-    <sheet name="meta" sheetId="3" r:id="rId2"/>
-    <sheet name="fish_data" sheetId="2" r:id="rId3"/>
+    <sheet name="fish_data" sheetId="2" r:id="rId2"/>
+    <sheet name="meta" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>location</t>
   </si>
@@ -67,22 +67,10 @@
     <t>shinydata/fromLiz/FWRI_KeyWest/16kHz_Decimated/Indices_Native_30sec/2020_03/Decimated_16kHzSR_512/Acoustic_Indices_16kHz_30sec_512_20_03.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">shinydata/fromLiz/FWRI_KeyWest/16kHz_Decimated/Indices_Native_30sec/2020_02/Decimated_16kHzSR_1024/Acoustic_Indices_16kHz_30sec_1024_20_02.csv"        </t>
+    <t>shinydata/fromLiz/FWRI_KeyWest/16kHz_Decimated/Indices_Native_30sec/2020_02/Decimated_16kHzSR_1024/Acoustic_Indices_16kHz_30sec_1024_20_02.csv</t>
   </si>
   <si>
     <t>shinydata/fromLiz/FWRI_KeyWest/16kHz_Decimated/Indices_Native_30sec/2020_03/Decimated_16kHzSR_1024/Acoustic_Indices_16kHz_30sec_1024_20_03.csv</t>
-  </si>
-  <si>
-    <t>shinydata/fromLiz/Chuckchi_Sea_AK/Indices_NativeDuration_25min/2019_02/Acoustic_Indices.csv</t>
-  </si>
-  <si>
-    <t>shinydata/fromLiz/Chuckchi_Sea_AK/Indices_NativeDuration_25min/2019_01/Acoustic_Indices.csv</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>chukchi</t>
   </si>
   <si>
     <t>keywest</t>
@@ -481,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B06102-E05E-E445-BAB6-1855B1811413}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,53 +505,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>16000</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>-1</v>
+        <v>1024</v>
       </c>
       <c r="E2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>16000</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>512</v>
       </c>
       <c r="E3">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>16000</v>
@@ -578,15 +566,15 @@
         <v>2020</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>16000</v>
@@ -601,55 +589,9 @@
         <v>2020</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>16000</v>
-      </c>
-      <c r="C6">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>1024</v>
-      </c>
-      <c r="E6">
-        <v>2020</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>16000</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-      <c r="D7">
-        <v>512</v>
-      </c>
-      <c r="E7">
-        <v>2020</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -659,11 +601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B7A0D2-0F9D-9041-A279-93B51016109E}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200265E0-8B1E-E241-A625-451A50F907FD}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,15 +615,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -690,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200265E0-8B1E-E241-A625-451A50F907FD}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B7A0D2-0F9D-9041-A279-93B51016109E}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,39 +670,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>